<commit_message>
Improve the tests structure WIP
</commit_message>
<xml_diff>
--- a/server/test/ParserTests/CSVFiles/molecules.xlsx
+++ b/server/test/ParserTests/CSVFiles/molecules.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sync\Documents\Fac\Semestre_5\Projet\glowing-octo-guacamole\server\test\CSVParserData\CSVFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sync\Documents\Fac\Semestre_5\Projet\glowing-octo-guacamole\server\test\ParserTests\CSVFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60BA54E1-ECFC-46BD-96E2-482A3EDE9FB3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B1600FD-8135-4162-93EA-2A7DABEA1F4F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1371,10 +1371,10 @@
   <dimension ref="A1:T171"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D73" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D56" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E1" sqref="E1:E1048576"/>
+      <selection pane="bottomRight" activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
change prettier line width=120
</commit_message>
<xml_diff>
--- a/server/test/ParserTests/CSVFiles/molecules.xlsx
+++ b/server/test/ParserTests/CSVFiles/molecules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sync\Documents\Fac\Semestre_5\Projet\glowing-octo-guacamole\server\test\ParserTests\CSVFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B1600FD-8135-4162-93EA-2A7DABEA1F4F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB4E4A1C-8AD0-401D-B96C-80A2F3E427BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="242">
   <si>
     <t>DCI</t>
   </si>
@@ -834,6 +834,9 @@
   </si>
   <si>
     <t>CEPHALOSPORINE DE 3EME      GENERATION</t>
+  </si>
+  <si>
+    <t>5-NITRO-IMIDAZOLES </t>
   </si>
 </sst>
 </file>
@@ -1371,10 +1374,10 @@
   <dimension ref="A1:T171"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D56" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F56" sqref="F56"/>
+      <selection pane="bottomRight" activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4490,7 +4493,7 @@
         <v>204</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>222</v>
+        <v>241</v>
       </c>
       <c r="I141" s="2" t="s">
         <v>216</v>

</xml_diff>